<commit_message>
all features working properly
</commit_message>
<xml_diff>
--- a/Exporturi excel/CL/export_consum_silviutanase-2020.xlsx
+++ b/Exporturi excel/CL/export_consum_silviutanase-2020.xlsx
@@ -1496,64 +1496,64 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1305</v>
+        <v>1315</v>
       </c>
       <c r="G13" t="n">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="H13" t="n">
         <v>1.40182</v>
       </c>
       <c r="I13" t="n">
-        <v>148.59292</v>
+        <v>162.61112</v>
       </c>
       <c r="J13" t="n">
-        <v>28.23265480000001</v>
+        <v>30.8961128</v>
       </c>
       <c r="K13" t="n">
-        <v>0.106</v>
+        <v>0.116</v>
       </c>
       <c r="L13" t="n">
         <v>6.05</v>
       </c>
       <c r="M13" t="n">
-        <v>0.6413</v>
+        <v>0.7018</v>
       </c>
       <c r="N13" t="n">
-        <v>0.121847</v>
+        <v>0.133342</v>
       </c>
       <c r="O13" t="n">
-        <v>0.106</v>
+        <v>0.116</v>
       </c>
       <c r="P13" t="n">
         <v>71.68059</v>
       </c>
       <c r="Q13" t="n">
-        <v>7.59814254</v>
+        <v>8.31494844</v>
       </c>
       <c r="R13" t="n">
-        <v>1.4436470826</v>
+        <v>1.5798402036</v>
       </c>
       <c r="S13" t="n">
-        <v>-106</v>
+        <v>-116</v>
       </c>
       <c r="T13" t="n">
         <v>0.90812</v>
       </c>
       <c r="U13" t="n">
-        <v>-96.26072000000001</v>
+        <v>-105.34192</v>
       </c>
       <c r="V13" t="n">
-        <v>-18.2895368</v>
+        <v>-20.0149648</v>
       </c>
       <c r="W13" t="n">
-        <v>60.57164254000001</v>
+        <v>66.28594843999998</v>
       </c>
       <c r="X13" t="n">
-        <v>11.5086120826</v>
+        <v>12.5943302036</v>
       </c>
       <c r="Y13" t="n">
-        <v>72.08025462260002</v>
+        <v>78.88027864359998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>